<commit_message>
Curso 03 - Aula 04 - Finalizada
</commit_message>
<xml_diff>
--- a/data/dimensoes/cliente/in/CADASTRO DE CLIENTES.xlsx
+++ b/data/dimensoes/cliente/in/CADASTRO DE CLIENTES.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMPO\ETL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F9010-0806-4BB2-A1C0-2127F47DA00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="132">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -428,31 +422,7 @@
     <t>CNPJ</t>
   </si>
   <si>
-    <t>DF</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>PR</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
     <t>R. Haddock Lobo, 17 - Salvador - MG</t>
-  </si>
-  <si>
-    <t>RJ</t>
   </si>
   <si>
     <t>R. Manguaba, 21  - Belo Horizonte - MG</t>
@@ -461,8 +431,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,34 +440,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9.6"/>
-      <color rgb="FF374151"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF374151"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7F7F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -505,31 +457,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFD9D9E3"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,18 +772,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,25 +793,24 @@
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3759651739</v>
       </c>
@@ -894,15 +826,8 @@
       <c r="E2">
         <v>280000</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="2" t="str">
-        <f>_xlfn.CONCAT("UODATE tb_cliente SET CIDADE = '",G2,"' WHERE CPF = '", A2,"';")</f>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '3759651739';</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>44257562749</v>
       </c>
@@ -918,15 +843,8 @@
       <c r="E3">
         <v>350000</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="2" t="str">
-        <f t="shared" ref="H3:H58" si="0">_xlfn.CONCAT("UODATE tb_cliente SET CIDADE = '",G3,"' WHERE CPF = '", A3,"';")</f>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '44257562749';</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8268254785</v>
       </c>
@@ -942,15 +860,8 @@
       <c r="E4">
         <v>320000</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '8268254785';</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3040980351</v>
       </c>
@@ -966,15 +877,8 @@
       <c r="E5">
         <v>1800000</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '3040980351';</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>621950777</v>
       </c>
@@ -990,15 +894,8 @@
       <c r="E6">
         <v>280000</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '621950777';</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>33726329749</v>
       </c>
@@ -1014,15 +911,8 @@
       <c r="E7">
         <v>380000</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '33726329749';</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9824868712</v>
       </c>
@@ -1030,7 +920,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
         <v>117</v>
@@ -1038,15 +928,8 @@
       <c r="E8">
         <v>600000</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '9824868712';</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2078365742</v>
       </c>
@@ -1062,15 +945,8 @@
       <c r="E9">
         <v>1200000</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '2078365742';</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9594349760</v>
       </c>
@@ -1086,15 +962,8 @@
       <c r="E10">
         <v>400000</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '9594349760';</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>91988802768</v>
       </c>
@@ -1110,15 +979,8 @@
       <c r="E11">
         <v>260000</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'PR' WHERE CPF = '91988802768';</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2379494746</v>
       </c>
@@ -1134,15 +996,8 @@
       <c r="E12">
         <v>450000</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '2379494746';</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2373471728</v>
       </c>
@@ -1158,15 +1013,8 @@
       <c r="E13">
         <v>380000</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '2373471728';</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>82236119704</v>
       </c>
@@ -1182,15 +1030,8 @@
       <c r="E14">
         <v>280000</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RS' WHERE CPF = '82236119704';</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43390129715</v>
       </c>
@@ -1206,15 +1047,8 @@
       <c r="E15">
         <v>320000</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RS' WHERE CPF = '43390129715';</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>29863333700</v>
       </c>
@@ -1230,15 +1064,8 @@
       <c r="E16">
         <v>220000</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '29863333700';</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7053899799</v>
       </c>
@@ -1254,15 +1081,8 @@
       <c r="E17">
         <v>380000</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '7053899799';</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>46619968791</v>
       </c>
@@ -1278,15 +1098,8 @@
       <c r="E18">
         <v>290000</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '46619968791';</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2930317701</v>
       </c>
@@ -1302,15 +1115,8 @@
       <c r="E19">
         <v>380000</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '2930317701';</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>76815463753</v>
       </c>
@@ -1326,15 +1132,8 @@
       <c r="E20">
         <v>250000</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '76815463753';</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31292046791</v>
       </c>
@@ -1350,15 +1149,8 @@
       <c r="E21">
         <v>360000</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '31292046791';</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6964705783</v>
       </c>
@@ -1366,7 +1158,7 @@
         <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
         <v>115</v>
@@ -1374,15 +1166,8 @@
       <c r="E22">
         <v>270000</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '6964705783';</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>72629274772</v>
       </c>
@@ -1398,15 +1183,8 @@
       <c r="E23">
         <v>1800000</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RS' WHERE CPF = '72629274772';</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12805717724</v>
       </c>
@@ -1422,15 +1200,8 @@
       <c r="E24">
         <v>400000</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '12805717724';</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>77842952787</v>
       </c>
@@ -1446,15 +1217,8 @@
       <c r="E25">
         <v>280000</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '77842952787';</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>80683215787</v>
       </c>
@@ -1470,15 +1234,8 @@
       <c r="E26">
         <v>350000</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '80683215787';</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>64113060797</v>
       </c>
@@ -1494,15 +1251,8 @@
       <c r="E27">
         <v>320000</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '64113060797';</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8664533776</v>
       </c>
@@ -1518,15 +1268,8 @@
       <c r="E28">
         <v>460000</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RS' WHERE CPF = '8664533776';</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>77126718772</v>
       </c>
@@ -1542,15 +1285,8 @@
       <c r="E29">
         <v>380000</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RJ' WHERE CPF = '77126718772';</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5194978723</v>
       </c>
@@ -1566,15 +1302,8 @@
       <c r="E30">
         <v>280000</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'PR' WHERE CPF = '5194978723';</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>64009319372</v>
       </c>
@@ -1590,15 +1319,8 @@
       <c r="E31">
         <v>420000</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RS' WHERE CPF = '64009319372';</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>82393222715</v>
       </c>
@@ -1614,15 +1336,8 @@
       <c r="E32">
         <v>290000</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'PR' WHERE CPF = '82393222715';</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>887713777</v>
       </c>
@@ -1638,15 +1353,8 @@
       <c r="E33">
         <v>380000</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '887713777';</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>13332132717</v>
       </c>
@@ -1662,15 +1370,8 @@
       <c r="E34">
         <v>1500000</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '13332132717';</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>49609165753</v>
       </c>
@@ -1686,15 +1387,8 @@
       <c r="E35">
         <v>400000</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'PR' WHERE CPF = '49609165753';</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10760990760</v>
       </c>
@@ -1710,15 +1404,8 @@
       <c r="E36">
         <v>280000</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '10760990760';</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10493761705</v>
       </c>
@@ -1734,15 +1421,8 @@
       <c r="E37">
         <v>350000</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RS' WHERE CPF = '10493761705';</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>75445719715</v>
       </c>
@@ -1758,15 +1438,8 @@
       <c r="E38">
         <v>320000</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '75445719715';</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11504339738</v>
       </c>
@@ -1782,15 +1455,8 @@
       <c r="E39">
         <v>240000</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '11504339738';</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38496275787</v>
       </c>
@@ -1806,15 +1472,8 @@
       <c r="E40">
         <v>380000</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RJ' WHERE CPF = '38496275787';</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>90830636749</v>
       </c>
@@ -1830,15 +1489,8 @@
       <c r="E41">
         <v>310000</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '90830636749';</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3760238300</v>
       </c>
@@ -1854,15 +1506,8 @@
       <c r="E42">
         <v>1200000</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'PR' WHERE CPF = '3760238300';</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5427963766</v>
       </c>
@@ -1878,15 +1523,8 @@
       <c r="E43">
         <v>380000</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '5427963766';</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>47268018720</v>
       </c>
@@ -1902,15 +1540,8 @@
       <c r="E44">
         <v>280000</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'GO' WHERE CPF = '47268018720';</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7150192793</v>
       </c>
@@ -1926,15 +1557,8 @@
       <c r="E45">
         <v>350000</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RJ' WHERE CPF = '7150192793';</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>87549999791</v>
       </c>
@@ -1950,15 +1574,8 @@
       <c r="E46">
         <v>320000</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '87549999791';</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>99010968715</v>
       </c>
@@ -1974,15 +1591,8 @@
       <c r="E47">
         <v>280000</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H47" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '99010968715';</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>25198076600</v>
       </c>
@@ -1998,15 +1608,8 @@
       <c r="E48">
         <v>400000</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H48" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MS' WHERE CPF = '25198076600';</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>78623359704</v>
       </c>
@@ -2022,15 +1625,8 @@
       <c r="E49">
         <v>300000</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H49" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '78623359704';</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7129236752</v>
       </c>
@@ -2046,15 +1642,8 @@
       <c r="E50">
         <v>1800000</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H50" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RJ' WHERE CPF = '7129236752';</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>44646550768</v>
       </c>
@@ -2070,15 +1659,8 @@
       <c r="E51">
         <v>400000</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H51" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '44646550768';</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>90005511704</v>
       </c>
@@ -2094,15 +1676,8 @@
       <c r="E52">
         <v>280000</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H52" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '90005511704';</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>84490438753</v>
       </c>
@@ -2118,15 +1693,8 @@
       <c r="E53">
         <v>350000</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H53" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'DF' WHERE CPF = '84490438753';</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>46118837449</v>
       </c>
@@ -2142,15 +1710,8 @@
       <c r="E54">
         <v>320000</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H54" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '46118837449';</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7317856738</v>
       </c>
@@ -2166,15 +1727,8 @@
       <c r="E55">
         <v>260000</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H55" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '7317856738';</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>30780411749</v>
       </c>
@@ -2190,15 +1744,8 @@
       <c r="E56">
         <v>380000</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H56" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'SP' WHERE CPF = '30780411749';</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>81034342720</v>
       </c>
@@ -2214,15 +1761,8 @@
       <c r="E57">
         <v>330000</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H57" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'RJ' WHERE CPF = '81034342720';</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>66631300720</v>
       </c>
@@ -2237,13 +1777,6 @@
       </c>
       <c r="E58">
         <v>250000</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UODATE tb_cliente SET CIDADE = 'MG' WHERE CPF = '66631300720';</v>
       </c>
     </row>
   </sheetData>

</xml_diff>